<commit_message>
cópia das abas de monitoramento/resumo - form 1,2,3
</commit_message>
<xml_diff>
--- a/outputs/belem_atualizado.xlsx
+++ b/outputs/belem_atualizado.xlsx
@@ -7,14 +7,15 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Form 1 - Município" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Form 2 - UVR" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Form 3 - Empreendimento" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Resumo" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Form 1 - Município" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Form 2 - UVR" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Form 3 - Empreendimento" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Form 1 - Município'!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Form 2 - UVR'!$A$1:$G$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Form 3 - Empreendimento'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Form 1 - Município'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Form 2 - UVR'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Form 3 - Empreendimento'!$A$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -23,13 +24,29 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="7">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <color theme="0"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <color theme="1"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="12"/>
     </font>
     <font>
       <name val="Arial"/>
@@ -47,12 +64,18 @@
       <sz val="11"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -79,13 +102,39 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -105,21 +154,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -565,306 +626,207 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="14" customWidth="1" min="1" max="1"/>
-    <col width="14" customWidth="1" min="2" max="2"/>
-    <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="32" customWidth="1" min="4" max="4"/>
-    <col width="13" customWidth="1" min="5" max="5"/>
-    <col width="18" customWidth="1" min="6" max="6"/>
-    <col width="27" customWidth="1" min="7" max="7"/>
-    <col width="16" customWidth="1" min="8" max="8"/>
-    <col width="34" customWidth="1" min="9" max="9"/>
-    <col width="25" customWidth="1" min="10" max="10"/>
-    <col width="26" customWidth="1" min="11" max="11"/>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="12.85546875" customWidth="1" min="2" max="2"/>
+    <col width="12.28515625" customWidth="1" min="3" max="3"/>
+    <col width="15.140625" customWidth="1" min="4" max="4"/>
+    <col width="12" customWidth="1" min="5" max="5"/>
+    <col width="15.140625" customWidth="1" min="6" max="6"/>
+    <col width="11.85546875" customWidth="1" min="7" max="7"/>
+    <col width="10.85546875" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" ht="18.75" customHeight="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>Regional</t>
+          <t>Formulário</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>Município</t>
+          <t>Enviados</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>UVR</t>
+          <t>%</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>Técnico de UVR</t>
+          <t>Atrasados</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Situação</t>
+          <t>%</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Data de Envio</t>
+          <t>Sem Técnico</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Validado pelo Regional</t>
+          <t>%</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>Observações</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Formulários para Deletar (ID)</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Validado Equip de TI</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Resposta Equipe de TI</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B2" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="D2" s="3" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
-      </c>
-      <c r="E2" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>25/05/2025</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="H2" s="3" t="n"/>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K2" s="3" t="n"/>
-    </row>
-    <row r="3">
+          <t>1 - Município</t>
+        </is>
+      </c>
+      <c r="B2" s="2">
+        <f>COUNTIF(INDIRECT("'Form 1 - Município'!E2:E100"),"Enviado")</f>
+        <v/>
+      </c>
+      <c r="C2" s="3">
+        <f>B2/SUM($B2,$D2,$F2)</f>
+        <v/>
+      </c>
+      <c r="D2" s="2">
+        <f>COUNTIF(INDIRECT("'Form 1 - Município'!E2:E100"),"Atrasado")</f>
+        <v/>
+      </c>
+      <c r="E2" s="3">
+        <f>D2/SUM($B2,$D2,$F2)</f>
+        <v/>
+      </c>
+      <c r="F2" s="2">
+        <f>COUNTIF(INDIRECT("'Form 1 - Município'!E2:E100"),"Sem Técnico")</f>
+        <v/>
+      </c>
+      <c r="G2" s="3">
+        <f>F2/SUM($B2,$D2,$F2)</f>
+        <v/>
+      </c>
+      <c r="H2" s="4">
+        <f>SUM(B2,D2,F2)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B3" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C3" s="3" t="n">
-        <v>2</v>
-      </c>
-      <c r="D3" s="3" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
-      </c>
-      <c r="E3" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>25/05/2025</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K3" s="3" t="n"/>
-    </row>
-    <row r="4">
+          <t>2 - UVR</t>
+        </is>
+      </c>
+      <c r="B3" s="2">
+        <f>COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Enviado")</f>
+        <v/>
+      </c>
+      <c r="C3" s="3">
+        <f>B3/SUM($B3,$D3,$F3)</f>
+        <v/>
+      </c>
+      <c r="D3" s="2">
+        <f>COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Atrasado")</f>
+        <v/>
+      </c>
+      <c r="E3" s="3">
+        <f>D3/SUM($B3,$D3,$F3)</f>
+        <v/>
+      </c>
+      <c r="F3" s="2">
+        <f>COUNTIF(INDIRECT("'Form 2 - UVR'!E2:E100"),"Sem Técnico")</f>
+        <v/>
+      </c>
+      <c r="G3" s="3">
+        <f>F3/SUM($B3,$D3,$F3)</f>
+        <v/>
+      </c>
+      <c r="H3" s="4">
+        <f>SUM(B3,D3,F3)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B4" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C4" s="3" t="n">
-        <v>3</v>
-      </c>
-      <c r="D4" s="3" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
-      </c>
-      <c r="E4" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>25/05/2025</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="H4" s="3" t="n"/>
-      <c r="I4" s="3" t="n"/>
-      <c r="J4" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K4" s="3" t="n"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Ana Paula</t>
-        </is>
-      </c>
-      <c r="B5" s="3" t="inlineStr">
-        <is>
-          <t>Belém</t>
-        </is>
-      </c>
-      <c r="C5" s="3" t="n">
-        <v>4</v>
-      </c>
-      <c r="D5" s="3" t="inlineStr">
-        <is>
-          <t>Thiago da Sailva Santos</t>
-        </is>
-      </c>
-      <c r="E5" s="4" t="inlineStr">
-        <is>
-          <t>Enviado</t>
-        </is>
-      </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>25/05/2025</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
-        <is>
-          <t>Sim</t>
-        </is>
-      </c>
-      <c r="H5" s="3" t="n"/>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="3" t="inlineStr">
-        <is>
-          <t>Não</t>
-        </is>
-      </c>
-      <c r="K5" s="3" t="n"/>
+          <t>3 - Empreendimento</t>
+        </is>
+      </c>
+      <c r="B4" s="2">
+        <f>COUNTIF(INDIRECT("'Form 3 - Empreendimento'!E2:E100"),"Enviado")</f>
+        <v/>
+      </c>
+      <c r="C4" s="3">
+        <f>B4/SUM($B4,$D4,$F4)</f>
+        <v/>
+      </c>
+      <c r="D4" s="2">
+        <f>COUNTIF(INDIRECT("'Form 3 - Empreendimento'!E2:E100"),"Atrasado")</f>
+        <v/>
+      </c>
+      <c r="E4" s="3">
+        <f>D4/SUM($B4,$D4,$F4)</f>
+        <v/>
+      </c>
+      <c r="F4" s="2">
+        <f>COUNTIF(INDIRECT("'Form 3 - Empreendimento'!E2:E100"),"Sem Técnico")</f>
+        <v/>
+      </c>
+      <c r="G4" s="3">
+        <f>F4/SUM($B4,$D4,$F4)</f>
+        <v/>
+      </c>
+      <c r="H4" s="4">
+        <f>SUM(B4,D4,F4)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="4" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+      <c r="B5" s="4">
+        <f>SUM(B2:B4)</f>
+        <v/>
+      </c>
+      <c r="C5" s="3">
+        <f>B5/SUM($B5,$D5,$F5)</f>
+        <v/>
+      </c>
+      <c r="D5" s="4">
+        <f>SUM(D2:D4)</f>
+        <v/>
+      </c>
+      <c r="E5" s="3">
+        <f>D5/SUM($B5,$D5,$F5)</f>
+        <v/>
+      </c>
+      <c r="F5" s="4">
+        <f>SUM(F2:F4)</f>
+        <v/>
+      </c>
+      <c r="G5" s="3">
+        <f>F5/SUM($B5,$D5,$F5)</f>
+        <v/>
+      </c>
+      <c r="H5" s="4">
+        <f>SUM(B5,D5,F5)</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:G1"/>
-  <conditionalFormatting sqref="G2:G5">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
-      <formula>"Sim"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
-      <formula>"Não"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J5">
-    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
-      <formula>"Sim"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
-      <formula>"Não"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
-      <formula>"Em Análise"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E5">
-    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
-      <formula>"Enviado"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
-      <formula>"Atrasado"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
-      <formula>"Outras Ocorrências"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
-      <formula>"Sem Técnico"</formula>
-    </cfRule>
-    <cfRule type="cellIs" priority="10" operator="equal" dxfId="5" stopIfTrue="1">
-      <formula>"Duplicado"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="3">
-    <dataValidation sqref="G2 G3 G4 G5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Sim,Não"</formula1>
-    </dataValidation>
-    <dataValidation sqref="J2 J3 J4 J5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Sim,Não, Em Análise"</formula1>
-    </dataValidation>
-    <dataValidation sqref="E2 E3 E4 E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Enviado, Atrasado, Outras Ocorrências, Sem Técnico, Duplicado"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -898,233 +860,233 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Regional</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Município</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>UVR</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Técnico de UVR</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Situação</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Data de Envio</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Validado pelo Regional</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Observações</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Formulários para Deletar (ID)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>Validado Equip de TI</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>Resposta Equipe de TI</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="7" t="inlineStr">
         <is>
           <t>Ana Luiza de Araujo e Silva</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
-        <is>
-          <t>18/12/2024</t>
-        </is>
-      </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="F2" s="7" t="inlineStr">
+        <is>
+          <t>25/05/2025</t>
+        </is>
+      </c>
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H2" s="3" t="n"/>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="inlineStr">
+      <c r="H2" s="7" t="n"/>
+      <c r="I2" s="7" t="n"/>
+      <c r="J2" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="7" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="7" t="inlineStr">
         <is>
           <t>Herlem Carlen Ferro</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
-        <is>
-          <t>27/12/2024</t>
-        </is>
-      </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>25/05/2025</t>
+        </is>
+      </c>
+      <c r="G3" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="3" t="inlineStr">
+      <c r="H3" s="7" t="n"/>
+      <c r="I3" s="7" t="n"/>
+      <c r="J3" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Monica Goreth Costa Ribeiro</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
-        <is>
-          <t>10/01/2025</t>
-        </is>
-      </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>25/05/2025</t>
+        </is>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H4" s="3" t="n"/>
-      <c r="I4" s="3" t="n"/>
-      <c r="J4" s="3" t="inlineStr">
+      <c r="H4" s="7" t="n"/>
+      <c r="I4" s="7" t="n"/>
+      <c r="J4" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="7" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="D5" s="7" t="inlineStr">
         <is>
           <t>Thiago da Sailva Santos</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="E5" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
-        <is>
-          <t>11/12/2024</t>
-        </is>
-      </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>25/05/2025</t>
+        </is>
+      </c>
+      <c r="G5" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H5" s="3" t="n"/>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="3" t="inlineStr">
+      <c r="H5" s="7" t="n"/>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="7" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>
@@ -1169,7 +1131,7 @@
       <formula1>"Sim,Não"</formula1>
     </dataValidation>
     <dataValidation sqref="J2 J3 J4 J5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"Sim,Não,Em Análise"</formula1>
+      <formula1>"Sim,Não, Em Análise"</formula1>
     </dataValidation>
     <dataValidation sqref="E2 E3 E4 E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
       <formula1>"Enviado, Atrasado, Outras Ocorrências, Sem Técnico, Duplicado"</formula1>
@@ -1208,233 +1170,543 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="5" t="inlineStr">
         <is>
           <t>Regional</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
         <is>
           <t>Município</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="C1" s="5" t="inlineStr">
         <is>
           <t>UVR</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="D1" s="5" t="inlineStr">
         <is>
           <t>Técnico de UVR</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="E1" s="5" t="inlineStr">
         <is>
           <t>Situação</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="F1" s="5" t="inlineStr">
         <is>
           <t>Data de Envio</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="G1" s="5" t="inlineStr">
         <is>
           <t>Validado pelo Regional</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="H1" s="5" t="inlineStr">
         <is>
           <t>Observações</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="I1" s="5" t="inlineStr">
         <is>
           <t>Formulários para Deletar (ID)</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="J1" s="5" t="inlineStr">
         <is>
           <t>Validado Equip de TI</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="K1" s="5" t="inlineStr">
         <is>
           <t>Resposta Equipe de TI</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="2" t="inlineStr">
+      <c r="A2" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B2" s="3" t="inlineStr">
+      <c r="B2" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C2" s="3" t="n">
+      <c r="C2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="3" t="inlineStr">
+      <c r="D2" s="7" t="inlineStr">
         <is>
           <t>Ana Luiza de Araujo e Silva</t>
         </is>
       </c>
-      <c r="E2" s="4" t="inlineStr">
+      <c r="E2" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F2" s="3" t="inlineStr">
+      <c r="F2" s="7" t="inlineStr">
+        <is>
+          <t>18/12/2024</t>
+        </is>
+      </c>
+      <c r="G2" s="9" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H2" s="7" t="n"/>
+      <c r="I2" s="7" t="n"/>
+      <c r="J2" s="7" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K2" s="7" t="n"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="6" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B3" s="7" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C3" s="7" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="7" t="inlineStr">
+        <is>
+          <t>Herlem Carlen Ferro</t>
+        </is>
+      </c>
+      <c r="E3" s="8" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F3" s="7" t="inlineStr">
+        <is>
+          <t>27/12/2024</t>
+        </is>
+      </c>
+      <c r="G3" s="9" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H3" s="7" t="n"/>
+      <c r="I3" s="7" t="n"/>
+      <c r="J3" s="7" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K3" s="7" t="n"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="6" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B4" s="7" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C4" s="7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" s="7" t="inlineStr">
+        <is>
+          <t>Monica Goreth Costa Ribeiro</t>
+        </is>
+      </c>
+      <c r="E4" s="8" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F4" s="7" t="inlineStr">
+        <is>
+          <t>10/01/2025</t>
+        </is>
+      </c>
+      <c r="G4" s="9" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H4" s="7" t="n"/>
+      <c r="I4" s="7" t="n"/>
+      <c r="J4" s="7" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K4" s="7" t="n"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="6" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B5" s="7" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C5" s="7" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="7" t="inlineStr">
+        <is>
+          <t>Thiago da Sailva Santos</t>
+        </is>
+      </c>
+      <c r="E5" s="8" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F5" s="7" t="inlineStr">
+        <is>
+          <t>11/12/2024</t>
+        </is>
+      </c>
+      <c r="G5" s="9" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
+      <c r="H5" s="7" t="n"/>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="inlineStr">
+        <is>
+          <t>Não</t>
+        </is>
+      </c>
+      <c r="K5" s="7" t="n"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G1"/>
+  <conditionalFormatting sqref="G2:G5">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+      <formula>"Sim"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+      <formula>"Não"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J5">
+    <cfRule type="cellIs" priority="1" operator="equal" dxfId="0" stopIfTrue="1">
+      <formula>"Sim"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" dxfId="1" stopIfTrue="1">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="5" operator="equal" dxfId="2" stopIfTrue="1">
+      <formula>"Em Análise"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E5">
+    <cfRule type="cellIs" priority="6" operator="equal" dxfId="3" stopIfTrue="1">
+      <formula>"Enviado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="equal" dxfId="4" stopIfTrue="1">
+      <formula>"Atrasado"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="8" operator="equal" dxfId="5" stopIfTrue="1">
+      <formula>"Outras Ocorrências"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" dxfId="6" stopIfTrue="1">
+      <formula>"Sem Técnico"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="equal" dxfId="5" stopIfTrue="1">
+      <formula>"Duplicado"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="3">
+    <dataValidation sqref="G2 G3 G4 G5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Sim,Não"</formula1>
+    </dataValidation>
+    <dataValidation sqref="J2 J3 J4 J5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Sim,Não,Em Análise"</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2 E3 E4 E5" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"Enviado, Atrasado, Outras Ocorrências, Sem Técnico, Duplicado"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane xSplit="3" topLeftCell="D1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="14" customWidth="1" min="1" max="1"/>
+    <col width="14" customWidth="1" min="2" max="2"/>
+    <col width="8" customWidth="1" min="3" max="3"/>
+    <col width="32" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="27" customWidth="1" min="7" max="7"/>
+    <col width="16" customWidth="1" min="8" max="8"/>
+    <col width="34" customWidth="1" min="9" max="9"/>
+    <col width="25" customWidth="1" min="10" max="10"/>
+    <col width="26" customWidth="1" min="11" max="11"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="5" t="inlineStr">
+        <is>
+          <t>Regional</t>
+        </is>
+      </c>
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>Município</t>
+        </is>
+      </c>
+      <c r="C1" s="5" t="inlineStr">
+        <is>
+          <t>UVR</t>
+        </is>
+      </c>
+      <c r="D1" s="5" t="inlineStr">
+        <is>
+          <t>Técnico de UVR</t>
+        </is>
+      </c>
+      <c r="E1" s="5" t="inlineStr">
+        <is>
+          <t>Situação</t>
+        </is>
+      </c>
+      <c r="F1" s="5" t="inlineStr">
+        <is>
+          <t>Data de Envio</t>
+        </is>
+      </c>
+      <c r="G1" s="5" t="inlineStr">
+        <is>
+          <t>Validado pelo Regional</t>
+        </is>
+      </c>
+      <c r="H1" s="5" t="inlineStr">
+        <is>
+          <t>Observações</t>
+        </is>
+      </c>
+      <c r="I1" s="5" t="inlineStr">
+        <is>
+          <t>Formulários para Deletar (ID)</t>
+        </is>
+      </c>
+      <c r="J1" s="5" t="inlineStr">
+        <is>
+          <t>Validado Equip de TI</t>
+        </is>
+      </c>
+      <c r="K1" s="5" t="inlineStr">
+        <is>
+          <t>Resposta Equipe de TI</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="6" t="inlineStr">
+        <is>
+          <t>Ana Paula</t>
+        </is>
+      </c>
+      <c r="B2" s="7" t="inlineStr">
+        <is>
+          <t>Belém</t>
+        </is>
+      </c>
+      <c r="C2" s="7" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="7" t="inlineStr">
+        <is>
+          <t>Ana Luiza de Araujo e Silva</t>
+        </is>
+      </c>
+      <c r="E2" s="8" t="inlineStr">
+        <is>
+          <t>Enviado</t>
+        </is>
+      </c>
+      <c r="F2" s="7" t="inlineStr">
         <is>
           <t>30/12/2024</t>
         </is>
       </c>
-      <c r="G2" s="5" t="inlineStr">
+      <c r="G2" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H2" s="3" t="n"/>
-      <c r="I2" s="3" t="n"/>
-      <c r="J2" s="3" t="inlineStr">
+      <c r="H2" s="7" t="n"/>
+      <c r="I2" s="7" t="n"/>
+      <c r="J2" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K2" s="3" t="n"/>
+      <c r="K2" s="7" t="n"/>
     </row>
     <row r="3">
-      <c r="A3" s="2" t="inlineStr">
+      <c r="A3" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B3" s="3" t="inlineStr">
+      <c r="B3" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="inlineStr">
+      <c r="D3" s="7" t="inlineStr">
         <is>
           <t>Herlem Carlen Ferro</t>
         </is>
       </c>
-      <c r="E3" s="4" t="inlineStr">
+      <c r="E3" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F3" s="3" t="inlineStr">
+      <c r="F3" s="7" t="inlineStr">
         <is>
           <t>18/12/2024</t>
         </is>
       </c>
-      <c r="G3" s="5" t="inlineStr">
+      <c r="G3" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H3" s="3" t="n"/>
-      <c r="I3" s="3" t="n"/>
-      <c r="J3" s="3" t="inlineStr">
+      <c r="H3" s="7" t="n"/>
+      <c r="I3" s="7" t="n"/>
+      <c r="J3" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K3" s="3" t="n"/>
+      <c r="K3" s="7" t="n"/>
     </row>
     <row r="4">
-      <c r="A4" s="2" t="inlineStr">
+      <c r="A4" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B4" s="3" t="inlineStr">
+      <c r="B4" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="3" t="inlineStr">
+      <c r="D4" s="7" t="inlineStr">
         <is>
           <t>Monica Goreth Costa Ribeiro</t>
         </is>
       </c>
-      <c r="E4" s="4" t="inlineStr">
+      <c r="E4" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F4" s="3" t="inlineStr">
+      <c r="F4" s="7" t="inlineStr">
         <is>
           <t>10/01/2025</t>
         </is>
       </c>
-      <c r="G4" s="5" t="inlineStr">
+      <c r="G4" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H4" s="3" t="n"/>
-      <c r="I4" s="3" t="n"/>
-      <c r="J4" s="3" t="inlineStr">
+      <c r="H4" s="7" t="n"/>
+      <c r="I4" s="7" t="n"/>
+      <c r="J4" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K4" s="3" t="n"/>
+      <c r="K4" s="7" t="n"/>
     </row>
     <row r="5">
-      <c r="A5" s="2" t="inlineStr">
+      <c r="A5" s="6" t="inlineStr">
         <is>
           <t>Ana Paula</t>
         </is>
       </c>
-      <c r="B5" s="3" t="inlineStr">
+      <c r="B5" s="7" t="inlineStr">
         <is>
           <t>Belém</t>
         </is>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="3" t="inlineStr">
+      <c r="D5" s="7" t="inlineStr">
         <is>
           <t>Thiago da Sailva Santos</t>
         </is>
       </c>
-      <c r="E5" s="4" t="inlineStr">
+      <c r="E5" s="8" t="inlineStr">
         <is>
           <t>Enviado</t>
         </is>
       </c>
-      <c r="F5" s="3" t="inlineStr">
+      <c r="F5" s="7" t="inlineStr">
         <is>
           <t>11/12/2024</t>
         </is>
       </c>
-      <c r="G5" s="5" t="inlineStr">
+      <c r="G5" s="9" t="inlineStr">
         <is>
           <t>Sim</t>
         </is>
       </c>
-      <c r="H5" s="3" t="n"/>
-      <c r="I5" s="3" t="n"/>
-      <c r="J5" s="3" t="inlineStr">
+      <c r="H5" s="7" t="n"/>
+      <c r="I5" s="7" t="n"/>
+      <c r="J5" s="7" t="inlineStr">
         <is>
           <t>Não</t>
         </is>
       </c>
-      <c r="K5" s="3" t="n"/>
+      <c r="K5" s="7" t="n"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:G1"/>

</xml_diff>

<commit_message>
Técnicos de UVR - Dinâmico
</commit_message>
<xml_diff>
--- a/outputs/belem_atualizado.xlsx
+++ b/outputs/belem_atualizado.xlsx
@@ -1159,7 +1159,7 @@
     <col width="14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="32" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
     <col width="27" customWidth="1" min="7" max="7"/>
@@ -1240,10 +1240,9 @@
       <c r="C2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
+      <c r="D2" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E2" s="8" t="inlineStr">
         <is>
@@ -1283,10 +1282,9 @@
       <c r="C3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
+      <c r="D3" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E3" s="8" t="inlineStr">
         <is>
@@ -1326,10 +1324,9 @@
       <c r="C4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
+      <c r="D4" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E4" s="8" t="inlineStr">
         <is>
@@ -1369,10 +1366,9 @@
       <c r="C5" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>Thiago da Sailva Santos</t>
-        </is>
+      <c r="D5" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>
@@ -1469,7 +1465,7 @@
     <col width="14" customWidth="1" min="1" max="1"/>
     <col width="14" customWidth="1" min="2" max="2"/>
     <col width="8" customWidth="1" min="3" max="3"/>
-    <col width="32" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="4" max="4"/>
     <col width="13" customWidth="1" min="5" max="5"/>
     <col width="18" customWidth="1" min="6" max="6"/>
     <col width="27" customWidth="1" min="7" max="7"/>
@@ -1550,10 +1546,9 @@
       <c r="C2" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="D2" s="7" t="inlineStr">
-        <is>
-          <t>Ana Luiza de Araujo e Silva</t>
-        </is>
+      <c r="D2" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B2&amp;C2, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E2" s="8" t="inlineStr">
         <is>
@@ -1593,10 +1588,9 @@
       <c r="C3" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="D3" s="7" t="inlineStr">
-        <is>
-          <t>Herlem Carlen Ferro</t>
-        </is>
+      <c r="D3" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B3&amp;C3, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E3" s="8" t="inlineStr">
         <is>
@@ -1636,10 +1630,9 @@
       <c r="C4" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="D4" s="7" t="inlineStr">
-        <is>
-          <t>Monica Goreth Costa Ribeiro</t>
-        </is>
+      <c r="D4" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B4&amp;C4, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E4" s="8" t="inlineStr">
         <is>
@@ -1679,10 +1672,9 @@
       <c r="C5" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="D5" s="7" t="inlineStr">
-        <is>
-          <t>Thiago da Sailva Santos</t>
-        </is>
+      <c r="D5" s="7">
+        <f>IFERROR(IF(INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))="", "", INDEX('Form 1 - Município'!D2:D500, MATCH(B5&amp;C5, INDEX('Form 1 - Município'!B2:B500&amp;'Form 1 - Município'!C2:C500, 0), 0))), "")</f>
+        <v/>
       </c>
       <c r="E5" s="8" t="inlineStr">
         <is>

</xml_diff>